<commit_message>
Houses Prices: 8 choose 2 2 2 2
</commit_message>
<xml_diff>
--- a/Houses Prices/NN_test_set_prediction_results_4_choose_2.xlsx
+++ b/Houses Prices/NN_test_set_prediction_results_4_choose_2.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yuval\Desktop\Data Science\Deconstructing Neural Networks\Houses Prices\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{338BB625-DE18-4249-A668-94351C72A6FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3491AED-8EE1-48A8-A05B-48D788037FB9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="180" windowWidth="25440" windowHeight="15390"/>
+    <workbookView xWindow="-25320" yWindow="180" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NN_test_set_prediction_results" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">NN_test_set_prediction_results!$A$1:$M$5</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>4 features</t>
   </si>
@@ -42,11 +55,29 @@
   <si>
     <t>['GrLivArea', 'GarageCars']</t>
   </si>
+  <si>
+    <t>Average MSE</t>
+  </si>
+  <si>
+    <t>Median MSE</t>
+  </si>
+  <si>
+    <t>Min MSE</t>
+  </si>
+  <si>
+    <t>Max MSE</t>
+  </si>
+  <si>
+    <t>group1</t>
+  </si>
+  <si>
+    <t>group2</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -183,7 +214,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -363,8 +394,14 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -479,6 +516,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -524,8 +576,14 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -880,159 +938,292 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="25.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="9" width="0" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C1">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="1">
         <v>0</v>
       </c>
-      <c r="D1">
+      <c r="D1" s="1">
         <v>1</v>
       </c>
-      <c r="E1">
+      <c r="E1" s="1">
         <v>2</v>
       </c>
-      <c r="F1">
+      <c r="F1" s="1">
         <v>3</v>
       </c>
-      <c r="G1">
+      <c r="G1" s="1">
         <v>4</v>
       </c>
-      <c r="H1">
+      <c r="H1" s="1">
         <v>5</v>
       </c>
-      <c r="I1">
+      <c r="I1" s="1">
         <v>6</v>
       </c>
+      <c r="J1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0.204326406121253</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0.205962374806404</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0.19553825259208599</v>
+      </c>
+      <c r="F2" s="2">
+        <v>0.210836827754974</v>
+      </c>
+      <c r="G2" s="2">
+        <v>0.20199069380760101</v>
+      </c>
+      <c r="H2" s="2">
+        <v>0.21369060873985199</v>
+      </c>
+      <c r="I2" s="2">
+        <v>0.196949481964111</v>
+      </c>
+      <c r="J2" s="2">
+        <f>AVERAGE(C2:I2)</f>
+        <v>0.20418494939804013</v>
+      </c>
+      <c r="K2" s="2">
+        <f>MEDIAN(C2:I2)</f>
+        <v>0.204326406121253</v>
+      </c>
+      <c r="L2" s="2">
+        <f>MIN(C2:I2)</f>
+        <v>0.19553825259208599</v>
+      </c>
+      <c r="M2" s="2">
+        <f>MAX(C2:I2)</f>
+        <v>0.21369060873985199</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2">
+      <c r="C3" s="2">
         <v>0.206943243741989</v>
       </c>
-      <c r="D2">
+      <c r="D3" s="2">
         <v>0.21229466795921301</v>
       </c>
-      <c r="E2">
+      <c r="E3" s="2">
         <v>0.205703139305114</v>
       </c>
-      <c r="F2">
+      <c r="F3" s="2">
         <v>0.210501834750175</v>
       </c>
-      <c r="G2">
+      <c r="G3" s="2">
         <v>0.20763920247554701</v>
       </c>
-      <c r="H2">
+      <c r="H3" s="2">
         <v>0.20354031026363301</v>
       </c>
-      <c r="I2">
+      <c r="I3" s="2">
         <v>0.201771259307861</v>
       </c>
+      <c r="J3" s="2">
+        <f>AVERAGE(C3:I3)</f>
+        <v>0.2069133796862189</v>
+      </c>
+      <c r="K3" s="2">
+        <f>MEDIAN(C3:I3)</f>
+        <v>0.206943243741989</v>
+      </c>
+      <c r="L3" s="2">
+        <f>MIN(C3:I3)</f>
+        <v>0.201771259307861</v>
+      </c>
+      <c r="M3" s="2">
+        <f>MAX(C3:I3)</f>
+        <v>0.21229466795921301</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C3">
+      <c r="C4" s="2">
         <v>0.216488808393478</v>
       </c>
-      <c r="D3">
+      <c r="D4" s="2">
         <v>0.21298058331012701</v>
       </c>
-      <c r="E3">
+      <c r="E4" s="2">
         <v>0.20725342631339999</v>
       </c>
-      <c r="F3">
+      <c r="F4" s="2">
         <v>0.22296743094921101</v>
       </c>
-      <c r="G3">
+      <c r="G4" s="2">
         <v>0.20808979868888799</v>
       </c>
-      <c r="H3">
+      <c r="H4" s="2">
         <v>0.21323430538177399</v>
       </c>
-      <c r="I3">
+      <c r="I4" s="2">
         <v>0.21788407862186401</v>
       </c>
+      <c r="J4" s="2">
+        <f>AVERAGE(C4:I4)</f>
+        <v>0.21412834737982031</v>
+      </c>
+      <c r="K4" s="2">
+        <f>MEDIAN(C4:I4)</f>
+        <v>0.21323430538177399</v>
+      </c>
+      <c r="L4" s="2">
+        <f>MIN(C4:I4)</f>
+        <v>0.20725342631339999</v>
+      </c>
+      <c r="M4" s="2">
+        <f>MAX(C4:I4)</f>
+        <v>0.22296743094921101</v>
+      </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4">
-        <v>0.204326406121253</v>
-      </c>
-      <c r="D4">
-        <v>0.205962374806404</v>
-      </c>
-      <c r="E4">
-        <v>0.19553825259208599</v>
-      </c>
-      <c r="F4">
-        <v>0.210836827754974</v>
-      </c>
-      <c r="G4">
-        <v>0.20199069380760101</v>
-      </c>
-      <c r="H4">
-        <v>0.21369060873985199</v>
-      </c>
-      <c r="I4">
-        <v>0.196949481964111</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="2">
         <v>0.194740414619445</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="2">
         <v>0.339570373296737</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="2">
         <v>0.209666952490806</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="2">
         <v>0.19576047360897</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="2">
         <v>0.21002662181854201</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="2">
         <v>0.212833002209663</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="2">
         <v>0.196144714951515</v>
+      </c>
+      <c r="J5" s="2">
+        <f>AVERAGE(C5:I5)</f>
+        <v>0.22267750757081115</v>
+      </c>
+      <c r="K5" s="2">
+        <f>MEDIAN(C5:I5)</f>
+        <v>0.209666952490806</v>
+      </c>
+      <c r="L5" s="2">
+        <f>MIN(C5:I5)</f>
+        <v>0.194740414619445</v>
+      </c>
+      <c r="M5" s="2">
+        <f>MAX(C5:I5)</f>
+        <v>0.339570373296737</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:M5" xr:uid="{24688429-5BF6-46C2-B75D-24209B20474D}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M5">
+      <sortCondition ref="J1:J5"/>
+    </sortState>
+  </autoFilter>
+  <conditionalFormatting sqref="J2:J5">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K2:K5">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L2:L5">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M2:M5">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>